<commit_message>
Update Rizka - Hapus Akun Bank
</commit_message>
<xml_diff>
--- a/DeleteAkunBank.xlsx
+++ b/DeleteAkunBank.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marvin\Documents\GitHub\ACC-Seamless-ACCOne\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY WORLD\KULIAH (TUGAS)\TGS SEMS. 8\INTERNSHIT\Task ACC ONE\ACC-ACCOne\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90FC96BF-DE8B-4E94-A6AF-0CBDE551F079}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{828CC53E-6386-481F-95F5-A4B589C5A676}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7635" yWindow="0" windowWidth="12330" windowHeight="11520" xr2:uid="{B07F0A7F-CE3E-4537-AD6C-B613D9BEF8B5}"/>
+    <workbookView xWindow="390" yWindow="0" windowWidth="13440" windowHeight="11070" xr2:uid="{B07F0A7F-CE3E-4537-AD6C-B613D9BEF8B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>NoRek</t>
   </si>
@@ -43,6 +43,18 @@
   </si>
   <si>
     <t>987654321</t>
+  </si>
+  <si>
+    <t>condition</t>
+  </si>
+  <si>
+    <t>passed</t>
+  </si>
+  <si>
+    <t>failed</t>
+  </si>
+  <si>
+    <t>utama</t>
   </si>
 </sst>
 </file>
@@ -58,15 +70,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -74,13 +98,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0F861E4-ACE0-4565-BFCA-1B70BE6DCAAB}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -406,40 +459,37 @@
     <col min="1" max="1" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
+      <c r="B2" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
+      <c r="B4" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>